<commit_message>
Actualizando los gráficos e incorporando visualización de embudo.
</commit_message>
<xml_diff>
--- a/output/Base_Final_Genero_Partidos.xlsx
+++ b/output/Base_Final_Genero_Partidos.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -493,6 +493,15 @@
       <c r="B7">
         <v>0.3225819816460547</v>
       </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.4459459459459459</v>
+      </c>
+      <c r="F7">
+        <v>0.3333333333333333</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -503,6 +512,18 @@
       <c r="B8">
         <v>0.4789527069861798</v>
       </c>
+      <c r="C8">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="D8">
+        <v>0.4523809523809524</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +632,15 @@
       <c r="B14">
         <v>0.4256155357762109</v>
       </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>0.4117647058823529</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -698,6 +728,18 @@
       <c r="B20">
         <v>0.5528716566452415</v>
       </c>
+      <c r="C20">
+        <v>0.6</v>
+      </c>
+      <c r="D20">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+      <c r="F20">
+        <v>0.4285714285714285</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -708,6 +750,15 @@
       <c r="B21">
         <v>0.482090067954083</v>
       </c>
+      <c r="C21">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D21">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -759,6 +810,18 @@
       <c r="B24">
         <v>0.2899685785302256</v>
       </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>0.4142857142857143</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0.1428571428571428</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -788,6 +851,18 @@
       <c r="B26">
         <v>0.4990123271572525</v>
       </c>
+      <c r="C26">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="D26">
+        <v>0.4418604651162791</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0.3076923076923077</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -825,130 +900,6 @@
       </c>
       <c r="D28">
         <v>0.4727272727272727</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>PARTIDO DE LA GENTE</t>
-        </is>
-      </c>
-      <c r="C29">
-        <v>0.5</v>
-      </c>
-      <c r="D29">
-        <v>0.4459459459459459</v>
-      </c>
-      <c r="F29">
-        <v>0.3333333333333333</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>PARTIDO DEMOCRATA CRISTIANO</t>
-        </is>
-      </c>
-      <c r="C30">
-        <v>0.4545454545454545</v>
-      </c>
-      <c r="D30">
-        <v>0.4523809523809524</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>PARTIDO LIBERAL DE CHILE</t>
-        </is>
-      </c>
-      <c r="C31">
-        <v>0.5</v>
-      </c>
-      <c r="D31">
-        <v>0.4117647058823529</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>PARTIDO POR LA DEMOCRACIA</t>
-        </is>
-      </c>
-      <c r="C32">
-        <v>0.6</v>
-      </c>
-      <c r="D32">
-        <v>0.4545454545454545</v>
-      </c>
-      <c r="E32">
-        <v>0.5</v>
-      </c>
-      <c r="F32">
-        <v>0.4285714285714285</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>PARTIDO RADICAL DE CHILE</t>
-        </is>
-      </c>
-      <c r="C33">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="D33">
-        <v>0.4642857142857143</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>PARTIDO REPUBLICANO DE CHILE</t>
-        </is>
-      </c>
-      <c r="C34">
-        <v>0.5</v>
-      </c>
-      <c r="D34">
-        <v>0.4142857142857143</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0.1428571428571428</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>PARTIDO SOCIALISTA DE CHILE</t>
-        </is>
-      </c>
-      <c r="C35">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="D35">
-        <v>0.4418604651162791</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0.3076923076923077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>